<commit_message>
arranged files for analysis closeness and degree
</commit_message>
<xml_diff>
--- a/inputs/b_emergence_check_new.xlsx
+++ b/inputs/b_emergence_check_new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzasenol/Desktop/Norm-Emergence/MAS/norm-changes-emergence/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64D308C5-9EBD-D643-B24C-9CA1347FB126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64A2CB8-8085-344F-B09D-0398FB6B02DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{EACB8860-D4BC-3A43-B2A2-974C31B8EA4F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="14">
   <si>
     <t>[0, 0, 1]</t>
   </si>
@@ -47,29 +47,44 @@
     <t>Epsilon</t>
   </si>
   <si>
-    <t>Trendsetter %</t>
-  </si>
-  <si>
     <t>Beta</t>
   </si>
   <si>
     <t>Weight</t>
   </si>
   <si>
-    <t>Trial</t>
-  </si>
-  <si>
-    <t>Percent of A</t>
-  </si>
-  <si>
-    <t>Percent of B</t>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>0.4</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>by degree</t>
+  </si>
+  <si>
+    <t>by closeness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trendsetter </t>
+  </si>
+  <si>
+    <t>Trendsetter Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +97,18 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,9 +131,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,15 +469,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D9D1A5-0C52-3043-8631-4F832DA98E8B}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:F81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -457,103 +485,79 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>100</v>
       </c>
       <c r="B2" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C2" s="1">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1">
-        <v>0.3</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C3" s="1">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0.3</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="1">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>100</v>
       </c>
       <c r="B4" s="1">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="C4" s="1">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.4</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="1">
-        <v>5</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>100</v>
       </c>
@@ -561,25 +565,19 @@
         <v>0.15</v>
       </c>
       <c r="C5" s="1">
-        <v>4</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.4</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="1">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>100</v>
       </c>
@@ -589,23 +587,17 @@
       <c r="C6" s="1">
         <v>10</v>
       </c>
-      <c r="D6" s="1">
-        <v>0.3</v>
+      <c r="D6" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="1">
-        <v>3</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>100</v>
       </c>
@@ -615,240 +607,435 @@
       <c r="C7" s="1">
         <v>10</v>
       </c>
-      <c r="D7" s="1">
-        <v>0.3</v>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="1">
-        <v>5</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>100</v>
       </c>
       <c r="B8" s="1">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C8" s="1">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0.3</v>
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="1">
-        <v>2</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>100</v>
       </c>
       <c r="B9" s="1">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C9" s="1">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0.3</v>
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>100</v>
       </c>
       <c r="B10" s="1">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C10" s="1">
-        <v>6</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0.4</v>
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="1">
-        <v>4</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>100</v>
       </c>
       <c r="B11" s="1">
-        <v>0.2</v>
+        <v>0.15</v>
       </c>
       <c r="C11" s="1">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0.4</v>
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="1">
-        <v>5</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>100</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C12" s="1">
-        <v>10</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>100</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C13" s="1">
-        <v>10</v>
-      </c>
-      <c r="D13" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>3</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>100</v>
-      </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>100</v>
-      </c>
-      <c r="B14" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="C14" s="1">
-        <v>10</v>
-      </c>
-      <c r="D14" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>100</v>
-      </c>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I25" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="1"/>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="1"/>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="2"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="2"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="2"/>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added new observation mechanism and added experiments
</commit_message>
<xml_diff>
--- a/inputs/b_emergence_check_new.xlsx
+++ b/inputs/b_emergence_check_new.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzasenol/Desktop/Norm-Emergence/MAS/norm-changes-emergence/inputs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beyzasenol/Desktop/norm-changes-emergence/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08AAFDA8-05DD-0445-9153-C148455436D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B80D7862-7B02-DD4C-9660-A9C27FE45F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16120" xr2:uid="{EACB8860-D4BC-3A43-B2A2-974C31B8EA4F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28420" windowHeight="16060" xr2:uid="{EACB8860-D4BC-3A43-B2A2-974C31B8EA4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="12">
   <si>
     <t>[0, 0, 1]</t>
   </si>
@@ -68,26 +68,17 @@
     <t>Trendsetter Type</t>
   </si>
   <si>
-    <t>[1, 0, 0]</t>
-  </si>
-  <si>
-    <t>[0, 1, 0]</t>
-  </si>
-  <si>
     <t>Topology</t>
   </si>
   <si>
     <t>scale_free</t>
-  </si>
-  <si>
-    <t>small_world</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -113,6 +104,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -134,10 +138,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,15 +478,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6D9D1A5-0C52-3043-8631-4F832DA98E8B}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="A1:J13"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,12 +509,12 @@
         <v>9</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B2" s="1">
         <v>0.15</v>
@@ -517,18 +526,18 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="B3" s="1">
         <v>0.15</v>
@@ -540,18 +549,18 @@
         <v>5</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="B4" s="1">
         <v>0.15</v>
@@ -563,18 +572,18 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="B5" s="1">
         <v>0.15</v>
@@ -586,18 +595,18 @@
         <v>5</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="B6" s="1">
         <v>0.15</v>
@@ -615,12 +624,12 @@
         <v>6</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>100</v>
+        <v>400</v>
       </c>
       <c r="B7" s="1">
         <v>0.15</v>
@@ -638,12 +647,12 @@
         <v>7</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="B8" s="1">
         <v>0.15</v>
@@ -655,18 +664,18 @@
         <v>5</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="B9" s="1">
         <v>0.15</v>
@@ -678,164 +687,129 @@
         <v>5</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>100</v>
-      </c>
-      <c r="B10" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="C10" s="1">
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>100</v>
-      </c>
-      <c r="B11" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="C11" s="1">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>100</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="C12" s="1">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>100</v>
-      </c>
-      <c r="B13" s="1">
-        <v>0.15</v>
-      </c>
-      <c r="C13" s="1">
-        <v>10</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="3"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="3"/>
       <c r="F17" s="2"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
+      <c r="E19" s="3"/>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="2"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="3"/>
+      <c r="H21" s="4"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -843,7 +817,7 @@
       <c r="E23" s="1"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -851,15 +825,7 @@
       <c r="E24" s="1"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="2"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -867,7 +833,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -875,7 +841,15 @@
       <c r="E27" s="1"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -883,15 +857,7 @@
       <c r="E29" s="1"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="2"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -899,13 +865,21 @@
       <c r="E31" s="1"/>
       <c r="F31" s="2"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
       <c r="E32" s="1"/>
       <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
@@ -915,14 +889,6 @@
       <c r="E34" s="1"/>
       <c r="F34" s="2"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="2"/>
-    </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
@@ -931,6 +897,14 @@
       <c r="E36" s="1"/>
       <c r="F36" s="2"/>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="2"/>
+    </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
@@ -939,30 +913,6 @@
       <c r="E38" s="1"/>
       <c r="F38" s="2"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="2"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="2"/>
-    </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
@@ -979,14 +929,6 @@
       <c r="E44" s="1"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="2"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="2"/>
-    </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
@@ -995,6 +937,14 @@
       <c r="E46" s="1"/>
       <c r="F46" s="2"/>
     </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="2"/>
+    </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
@@ -1019,93 +969,37 @@
       <c r="E50" s="1"/>
       <c r="F50" s="2"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="2"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="2"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="2"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="2"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="2"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="2"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="2"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="2"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="2"/>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="2"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="2"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>